<commit_message>
code for extracting additional clinical trials part AEs
</commit_message>
<xml_diff>
--- a/AE_to_MedDRA/Updated Files/Updated_Adakveo_06262024.xlsx
+++ b/AE_to_MedDRA/Updated Files/Updated_Adakveo_06262024.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -392,12 +392,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Infusion-related reactions</t>
+          <t>Arthralgia</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Bullet point</t>
+          <t>Table1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -408,13 +408,23 @@
       <c r="D2" t="inlineStr">
         <is>
           <t>NA</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>10003239</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>10003239</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Arthralgia</t>
+          <t>Nausea</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -434,19 +444,19 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>10003239</t>
+          <t>10028813</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>10003239</t>
+          <t>10028813</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Nausea</t>
+          <t>Back pain</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -466,19 +476,19 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>10028813</t>
+          <t>10003988</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>10028813</t>
+          <t>10003988</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Back pain</t>
+          <t>Abdominal pain</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -498,19 +508,19 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>10003988</t>
+          <t>10000081</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>10003988</t>
+          <t>10000081</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Abdominal pain</t>
+          <t>Pyrexia</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -530,19 +540,19 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>10000081</t>
+          <t>10037660</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>10000081</t>
+          <t>10037660</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Pyrexia</t>
+          <t>Diarrhea</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -562,42 +572,10 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>10037660</t>
+          <t>10012727</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
-        <is>
-          <t>10037660</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Diarrhea</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Table1</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>10012727</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
         <is>
           <t>10012735</t>
         </is>

</xml_diff>